<commit_message>
Tudo pronto para o semestre!
</commit_message>
<xml_diff>
--- a/content/plano-de-aulas.xlsx
+++ b/content/plano-de-aulas.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="102">
   <si>
     <t xml:space="preserve">Data</t>
   </si>
@@ -90,6 +90,9 @@
 </t>
   </si>
   <si>
+    <t xml:space="preserve">Rever testes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Comparando desempenho de algoritmos</t>
   </si>
   <si>
@@ -142,6 +145,9 @@
 Implementação do algoritmo usando testes de unidade.</t>
   </si>
   <si>
+    <t xml:space="preserve">Refazer</t>
+  </si>
+  <si>
     <t xml:space="preserve">Revisão Geral</t>
   </si>
   <si>
@@ -155,6 +161,9 @@
   </si>
   <si>
     <t xml:space="preserve">SEMANA AI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Criar do zero</t>
   </si>
   <si>
     <t xml:space="preserve">Recursão</t>
@@ -174,6 +183,9 @@
   <si>
     <t xml:space="preserve">Representação do Labirinto usando Matriz
 "Algoritmo da mão direita": desenvolver método inicial para sair do labirinto e implementar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisão leve</t>
   </si>
   <si>
     <t xml:space="preserve">Como encontrar um caminho até o destino?</t>
@@ -196,12 +208,18 @@
 Aluno faz implementação com testes de unidade</t>
   </si>
   <si>
+    <t xml:space="preserve">Revisão leve → encontrar problemas leetcode para ajudar na prática</t>
+  </si>
+  <si>
     <t xml:space="preserve">Estruturas de Dados</t>
   </si>
   <si>
     <t xml:space="preserve">Expositiva: algoritmos de encontrar todas as ocorrências + interface para o tipo Lista
 Handout: tipo List usando vetor dinâmico
 Implementação: vetor dinâmico em Java (tipo InsperList)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revisão leve → acertar discurso com ordem do curso</t>
   </si>
   <si>
     <t xml:space="preserve">Implementações de algoritmos com tipo lista
@@ -432,7 +450,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -467,6 +485,18 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.7999"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF38"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF9C0006"/>
       </patternFill>
     </fill>
   </fills>
@@ -546,7 +576,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -583,8 +613,16 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -658,7 +696,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFFF38"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF9C0006"/>
@@ -893,8 +931,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1016,49 +1054,56 @@
       <c r="F5" s="8" t="s">
         <v>18</v>
       </c>
+      <c r="G5" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
         <f aca="false">A4+7</f>
         <v>45525</v>
       </c>
-      <c r="B6" s="9" t="n">
+      <c r="B6" s="10" t="n">
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="0"/>
-      <c r="I6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
         <f aca="false">A5+7</f>
         <v>45527</v>
       </c>
-      <c r="B7" s="9" t="n">
+      <c r="B7" s="10" t="n">
         <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1066,24 +1111,24 @@
         <f aca="false">A6+7</f>
         <v>45532</v>
       </c>
-      <c r="B8" s="9" t="n">
+      <c r="B8" s="10" t="n">
         <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="0"/>
-      <c r="H8" s="0"/>
-      <c r="I8" s="0"/>
+        <v>26</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="65.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
@@ -1094,20 +1139,20 @@
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="0"/>
-      <c r="H9" s="0"/>
-      <c r="I9" s="0"/>
+        <v>28</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
@@ -1118,20 +1163,20 @@
         <v>8</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="0"/>
-      <c r="H10" s="0"/>
-      <c r="I10" s="0"/>
+        <v>31</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="99.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="n">
@@ -1142,123 +1187,121 @@
         <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="0"/>
-      <c r="H11" s="0"/>
-      <c r="I11" s="0"/>
+        <v>33</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
         <f aca="false">A10+7</f>
         <v>45546</v>
       </c>
-      <c r="B12" s="9" t="n">
+      <c r="B12" s="10" t="n">
         <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="0"/>
-      <c r="I12" s="0"/>
+        <v>38</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="n">
         <f aca="false">A11+7</f>
         <v>45548</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="10"/>
-      <c r="H13" s="0"/>
-      <c r="I13" s="0"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="12"/>
     </row>
     <row r="14" customFormat="false" ht="81.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="n">
         <f aca="false">A12+7</f>
         <v>45553</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="10"/>
-      <c r="H14" s="0"/>
-      <c r="I14" s="0"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="12"/>
     </row>
     <row r="15" customFormat="false" ht="103.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
         <f aca="false">A13+7</f>
         <v>45555</v>
       </c>
-      <c r="B15" s="9" t="n">
+      <c r="B15" s="10" t="n">
         <v>11</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" s="0"/>
-      <c r="I15" s="0"/>
+        <v>33</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
         <f aca="false">A14+7</f>
         <v>45560</v>
       </c>
-      <c r="B16" s="9" t="n">
+      <c r="B16" s="10" t="n">
         <v>12</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="11" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1267,20 +1310,23 @@
         <f aca="false">A15+7</f>
         <v>45562</v>
       </c>
-      <c r="B17" s="9" t="n">
+      <c r="B17" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>41</v>
+      <c r="C17" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E17" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1288,23 +1334,23 @@
         <f aca="false">A16+7</f>
         <v>45567</v>
       </c>
-      <c r="B18" s="9" t="n">
+      <c r="B18" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>41</v>
+      <c r="C18" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="45.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="n">
         <f aca="false">A17+7</f>
         <v>45569</v>
@@ -1312,17 +1358,20 @@
       <c r="B19" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>41</v>
+      <c r="C19" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>45</v>
+        <v>49</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="112.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1330,83 +1379,86 @@
         <f aca="false">A18+7</f>
         <v>45574</v>
       </c>
-      <c r="B20" s="9" t="n">
+      <c r="B20" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="C20" s="12" t="s">
-        <v>41</v>
+      <c r="C20" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="99.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="n">
         <f aca="false">A19+7</f>
         <v>45576</v>
       </c>
-      <c r="B21" s="9" t="n">
+      <c r="B21" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>41</v>
+      <c r="C21" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E21" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="94" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="112.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="n">
         <f aca="false">A20+7</f>
         <v>45581</v>
       </c>
-      <c r="B22" s="9" t="n">
+      <c r="B22" s="10" t="n">
         <v>18</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>41</v>
+      <c r="C22" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="106.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="n">
         <f aca="false">A21+7</f>
         <v>45583</v>
       </c>
-      <c r="B23" s="9" t="n">
+      <c r="B23" s="10" t="n">
         <v>19</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>41</v>
+      <c r="C23" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="94" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1414,20 +1466,20 @@
         <f aca="false">A22+7</f>
         <v>45588</v>
       </c>
-      <c r="B24" s="9" t="n">
+      <c r="B24" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>41</v>
+      <c r="C24" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E24" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1435,11 +1487,11 @@
         <f aca="false">A23+7</f>
         <v>45590</v>
       </c>
-      <c r="B25" s="9" t="n">
+      <c r="B25" s="10" t="n">
         <v>21</v>
       </c>
-      <c r="C25" s="13" t="s">
-        <v>49</v>
+      <c r="C25" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>14</v>
@@ -1448,7 +1500,10 @@
         <v>9</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>50</v>
+        <v>55</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1459,8 +1514,8 @@
       <c r="B26" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="C26" s="13" t="s">
-        <v>49</v>
+      <c r="C26" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>14</v>
@@ -1469,7 +1524,7 @@
         <v>9</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1480,17 +1535,17 @@
       <c r="B27" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="C27" s="13" t="s">
-        <v>49</v>
+      <c r="C27" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1501,17 +1556,17 @@
       <c r="B28" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>33</v>
+      <c r="C28" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1519,30 +1574,30 @@
         <f aca="false">A27+7</f>
         <v>45604</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="n">
         <f aca="false">A28+7</f>
         <v>45609</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1656,13 +1711,13 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>56</v>
+        <v>62</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>62</v>
       </c>
       <c r="F4" s="6"/>
     </row>
@@ -1674,7 +1729,7 @@
       <c r="B5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="15" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1692,10 +1747,10 @@
         <f aca="false">A4+7</f>
         <v>45343</v>
       </c>
-      <c r="B6" s="9" t="n">
+      <c r="B6" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -1713,20 +1768,20 @@
         <f aca="false">A5+7</f>
         <v>45345</v>
       </c>
-      <c r="B7" s="9" t="n">
+      <c r="B7" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1734,11 +1789,11 @@
         <f aca="false">A6+7</f>
         <v>45350</v>
       </c>
-      <c r="B8" s="9" t="n">
+      <c r="B8" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>49</v>
+      <c r="C8" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>14</v>
@@ -1747,7 +1802,7 @@
         <v>9</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="155.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1758,8 +1813,8 @@
       <c r="B9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>49</v>
+      <c r="C9" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>14</v>
@@ -1768,7 +1823,7 @@
         <v>9</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1779,17 +1834,17 @@
       <c r="B10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>49</v>
+      <c r="C10" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="99.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1801,7 +1856,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>14</v>
@@ -1810,7 +1865,7 @@
         <v>9</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1818,20 +1873,20 @@
         <f aca="false">A10+7</f>
         <v>45364</v>
       </c>
-      <c r="B12" s="9" t="n">
+      <c r="B12" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>21</v>
+      <c r="C12" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1839,18 +1894,18 @@
         <f aca="false">A11+7</f>
         <v>45366</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="12" t="s">
-        <v>21</v>
+      <c r="B13" s="12"/>
+      <c r="C13" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="81.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1858,18 +1913,18 @@
         <f aca="false">A12+7</f>
         <v>45371</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="12" t="s">
-        <v>33</v>
+      <c r="B14" s="12"/>
+      <c r="C14" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="103.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1877,55 +1932,55 @@
         <f aca="false">A13+7</f>
         <v>45373</v>
       </c>
-      <c r="B15" s="9" t="n">
+      <c r="B15" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="10"/>
+      <c r="C15" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
         <f aca="false">A14+7</f>
         <v>45378</v>
       </c>
-      <c r="B16" s="9" t="n">
+      <c r="B16" s="10" t="n">
         <v>12</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="10"/>
+      <c r="C16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="12"/>
     </row>
     <row r="17" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="n">
         <f aca="false">A15+7</f>
         <v>45380</v>
       </c>
-      <c r="B17" s="9" t="n">
+      <c r="B17" s="10" t="n">
         <v>13</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>56</v>
+        <v>62</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>62</v>
       </c>
       <c r="F17" s="6"/>
     </row>
@@ -1934,20 +1989,20 @@
         <f aca="false">A16+7</f>
         <v>45385</v>
       </c>
-      <c r="B18" s="9" t="n">
+      <c r="B18" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>21</v>
+      <c r="C18" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1958,17 +2013,17 @@
       <c r="B19" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>21</v>
+      <c r="C19" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1976,20 +2031,20 @@
         <f aca="false">A18+7</f>
         <v>45392</v>
       </c>
-      <c r="B20" s="9" t="n">
+      <c r="B20" s="10" t="n">
         <v>16</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1997,20 +2052,20 @@
         <f aca="false">A19+7</f>
         <v>45394</v>
       </c>
-      <c r="B21" s="9" t="n">
+      <c r="B21" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>41</v>
+      <c r="C21" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="94" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2018,20 +2073,20 @@
         <f aca="false">A20+7</f>
         <v>45399</v>
       </c>
-      <c r="B22" s="9" t="n">
+      <c r="B22" s="10" t="n">
         <v>18</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>41</v>
+      <c r="C22" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2039,20 +2094,20 @@
         <f aca="false">A21+7</f>
         <v>45401</v>
       </c>
-      <c r="B23" s="9" t="n">
+      <c r="B23" s="10" t="n">
         <v>19</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>41</v>
+      <c r="C23" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="94" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2060,20 +2115,20 @@
         <f aca="false">A22+7</f>
         <v>45406</v>
       </c>
-      <c r="B24" s="9" t="n">
+      <c r="B24" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>41</v>
+      <c r="C24" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2081,20 +2136,20 @@
         <f aca="false">A23+7</f>
         <v>45408</v>
       </c>
-      <c r="B25" s="9" t="n">
+      <c r="B25" s="10" t="n">
         <v>21</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>41</v>
+      <c r="C25" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2106,13 +2161,13 @@
         <v>22</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>56</v>
+        <v>62</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>62</v>
       </c>
       <c r="F26" s="6"/>
     </row>
@@ -2124,17 +2179,17 @@
       <c r="B27" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="C27" s="13" t="s">
-        <v>28</v>
+      <c r="C27" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2145,17 +2200,17 @@
       <c r="B28" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>28</v>
+      <c r="C28" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2163,30 +2218,30 @@
         <f aca="false">A27+7</f>
         <v>45422</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="n">
         <f aca="false">A28+7</f>
         <v>45427</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2300,13 +2355,13 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>56</v>
+        <v>62</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>62</v>
       </c>
       <c r="F4" s="6"/>
     </row>
@@ -2330,8 +2385,8 @@
       <c r="F5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="15" t="s">
-        <v>61</v>
+      <c r="G5" s="17" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2339,20 +2394,20 @@
         <f aca="false">A4+7</f>
         <v>45343</v>
       </c>
-      <c r="B6" s="9" t="n">
+      <c r="B6" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2360,10 +2415,10 @@
         <f aca="false">A5+7</f>
         <v>45345</v>
       </c>
-      <c r="B7" s="9" t="n">
+      <c r="B7" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="8" t="s">
@@ -2373,7 +2428,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2381,20 +2436,20 @@
         <f aca="false">A6+7</f>
         <v>45350</v>
       </c>
-      <c r="B8" s="9" t="n">
+      <c r="B8" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="155.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2405,8 +2460,8 @@
       <c r="B9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>67</v>
+      <c r="C9" s="15" t="s">
+        <v>73</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>14</v>
@@ -2426,8 +2481,8 @@
       <c r="B10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>67</v>
+      <c r="C10" s="15" t="s">
+        <v>73</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>14</v>
@@ -2436,7 +2491,7 @@
         <v>9</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="88.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2447,17 +2502,17 @@
       <c r="B11" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>67</v>
+      <c r="C11" s="15" t="s">
+        <v>73</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2465,11 +2520,11 @@
         <f aca="false">A10+7</f>
         <v>45364</v>
       </c>
-      <c r="B12" s="9" t="n">
+      <c r="B12" s="10" t="n">
         <v>10</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>14</v>
@@ -2478,7 +2533,7 @@
         <v>9</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2486,18 +2541,18 @@
         <f aca="false">A11+7</f>
         <v>45366</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="12" t="s">
-        <v>21</v>
+      <c r="B13" s="12"/>
+      <c r="C13" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="81.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2505,21 +2560,21 @@
         <f aca="false">A12+7</f>
         <v>45371</v>
       </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="12" t="s">
-        <v>21</v>
+      <c r="B14" s="12"/>
+      <c r="C14" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="103.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2527,49 +2582,49 @@
         <f aca="false">A13+7</f>
         <v>45373</v>
       </c>
-      <c r="B15" s="9" t="n">
+      <c r="B15" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F15" s="10"/>
+      <c r="C15" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
         <f aca="false">A14+7</f>
         <v>45378</v>
       </c>
-      <c r="B16" s="9" t="n">
+      <c r="B16" s="10" t="n">
         <v>12</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="10"/>
+      <c r="C16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="12"/>
       <c r="I16" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="J16" s="13" t="s">
-        <v>73</v>
+      <c r="J16" s="15" t="s">
+        <v>79</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2577,17 +2632,17 @@
         <f aca="false">A15+7</f>
         <v>45380</v>
       </c>
-      <c r="B17" s="9" t="n">
+      <c r="B17" s="10" t="n">
         <v>13</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>56</v>
+        <v>62</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>62</v>
       </c>
       <c r="F17" s="6"/>
     </row>
@@ -2596,20 +2651,20 @@
         <f aca="false">A16+7</f>
         <v>45385</v>
       </c>
-      <c r="B18" s="9" t="n">
+      <c r="B18" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="C18" s="12" t="s">
-        <v>21</v>
+      <c r="C18" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2620,17 +2675,17 @@
       <c r="B19" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>21</v>
+      <c r="C19" s="14" t="s">
+        <v>22</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2638,20 +2693,20 @@
         <f aca="false">A18+7</f>
         <v>45392</v>
       </c>
-      <c r="B20" s="9" t="n">
+      <c r="B20" s="10" t="n">
         <v>16</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2659,20 +2714,20 @@
         <f aca="false">A19+7</f>
         <v>45394</v>
       </c>
-      <c r="B21" s="9" t="n">
+      <c r="B21" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>41</v>
+      <c r="C21" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2680,23 +2735,23 @@
         <f aca="false">A20+7</f>
         <v>45399</v>
       </c>
-      <c r="B22" s="9" t="n">
+      <c r="B22" s="10" t="n">
         <v>18</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>41</v>
+      <c r="C22" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>61</v>
+        <v>49</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2704,20 +2759,20 @@
         <f aca="false">A21+7</f>
         <v>45401</v>
       </c>
-      <c r="B23" s="9" t="n">
+      <c r="B23" s="10" t="n">
         <v>19</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>41</v>
+      <c r="C23" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2725,20 +2780,20 @@
         <f aca="false">A22+7</f>
         <v>45406</v>
       </c>
-      <c r="B24" s="9" t="n">
+      <c r="B24" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>41</v>
+      <c r="C24" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2746,23 +2801,23 @@
         <f aca="false">A23+7</f>
         <v>45408</v>
       </c>
-      <c r="B25" s="9" t="n">
+      <c r="B25" s="10" t="n">
         <v>21</v>
       </c>
-      <c r="C25" s="12" t="s">
-        <v>41</v>
+      <c r="C25" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>61</v>
+        <v>50</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2774,13 +2829,13 @@
         <v>22</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>56</v>
+        <v>62</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>62</v>
       </c>
       <c r="F26" s="6"/>
     </row>
@@ -2792,17 +2847,17 @@
       <c r="B27" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="C27" s="13" t="s">
-        <v>28</v>
+      <c r="C27" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2813,20 +2868,20 @@
       <c r="B28" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>28</v>
+      <c r="C28" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>76</v>
+        <v>33</v>
+      </c>
+      <c r="G28" s="17" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2834,30 +2889,30 @@
         <f aca="false">A27+7</f>
         <v>45422</v>
       </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="n">
         <f aca="false">A28+7</f>
         <v>45427</v>
       </c>
-      <c r="B30" s="10"/>
-      <c r="C30" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2968,8 +3023,8 @@
       <c r="E4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>77</v>
+      <c r="F4" s="18" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2977,17 +3032,17 @@
         <f aca="false">A3+7</f>
         <v>44974</v>
       </c>
-      <c r="B5" s="9" t="n">
+      <c r="B5" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>78</v>
+      <c r="C5" s="19" t="s">
+        <v>84</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2996,7 +3051,7 @@
         <v>44979</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -3007,15 +3062,15 @@
         <f aca="false">A5+7</f>
         <v>44981</v>
       </c>
-      <c r="B7" s="9" t="n">
+      <c r="B7" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="8" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="102" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3023,15 +3078,15 @@
         <f aca="false">A6+7</f>
         <v>44986</v>
       </c>
-      <c r="B8" s="9" t="n">
+      <c r="B8" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="8" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="155.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3042,14 +3097,14 @@
       <c r="B9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="18" t="s">
-        <v>84</v>
+      <c r="C9" s="20" t="s">
+        <v>90</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3060,12 +3115,12 @@
       <c r="B10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="18"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="88.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3073,17 +3128,17 @@
         <f aca="false">A9+7</f>
         <v>44995</v>
       </c>
-      <c r="B11" s="9" t="n">
-        <v>9</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>21</v>
+      <c r="B11" s="10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>22</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3091,15 +3146,15 @@
         <f aca="false">A10+7</f>
         <v>45000</v>
       </c>
-      <c r="B12" s="9" t="n">
+      <c r="B12" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="C12" s="19"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3107,15 +3162,15 @@
         <f aca="false">A11+7</f>
         <v>45002</v>
       </c>
-      <c r="B13" s="9" t="n">
+      <c r="B13" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="C13" s="19"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3123,35 +3178,35 @@
         <f aca="false">A12+7</f>
         <v>45007</v>
       </c>
-      <c r="B14" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
+      <c r="B14" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
     </row>
     <row r="15" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
         <f aca="false">A13+7</f>
         <v>45009</v>
       </c>
-      <c r="B15" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
+      <c r="B15" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
         <f aca="false">A14+7</f>
         <v>45014</v>
       </c>
-      <c r="B16" s="9" t="n">
+      <c r="B16" s="10" t="n">
         <v>12</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>67</v>
+      <c r="C16" s="19" t="s">
+        <v>73</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>14</v>
@@ -3162,17 +3217,17 @@
       <c r="H16" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="I16" s="13" t="s">
-        <v>73</v>
+      <c r="I16" s="15" t="s">
+        <v>79</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="L16" s="16" t="s">
-        <v>77</v>
+        <v>81</v>
+      </c>
+      <c r="L16" s="18" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3180,15 +3235,15 @@
         <f aca="false">A15+7</f>
         <v>45016</v>
       </c>
-      <c r="B17" s="9" t="n">
+      <c r="B17" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="C17" s="17"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="21" t="s">
-        <v>88</v>
+      <c r="E17" s="23" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3197,7 +3252,7 @@
         <v>45021</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -3209,7 +3264,7 @@
         <v>45023</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -3220,18 +3275,18 @@
         <f aca="false">A18+7</f>
         <v>45028</v>
       </c>
-      <c r="B20" s="9" t="n">
+      <c r="B20" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="C20" s="17"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="8" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>77</v>
+        <v>95</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3243,13 +3298,13 @@
         <v>15</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3262,10 +3317,10 @@
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3274,7 +3329,7 @@
         <v>45037</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -3290,10 +3345,10 @@
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3306,10 +3361,10 @@
       </c>
       <c r="C25" s="7"/>
       <c r="D25" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3317,17 +3372,17 @@
         <f aca="false">A24+7</f>
         <v>45049</v>
       </c>
-      <c r="B26" s="9" t="n">
+      <c r="B26" s="10" t="n">
         <v>19</v>
       </c>
-      <c r="C26" s="19" t="s">
-        <v>94</v>
+      <c r="C26" s="21" t="s">
+        <v>100</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3335,13 +3390,13 @@
         <f aca="false">A25+7</f>
         <v>45051</v>
       </c>
-      <c r="B27" s="9" t="n">
+      <c r="B27" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="9"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="10"/>
       <c r="E27" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3349,13 +3404,13 @@
         <f aca="false">A26+7</f>
         <v>45056</v>
       </c>
-      <c r="B28" s="9" t="n">
+      <c r="B28" s="10" t="n">
         <v>21</v>
       </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="9"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="10"/>
       <c r="E28" s="8" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3363,12 +3418,12 @@
         <f aca="false">A27+7</f>
         <v>45058</v>
       </c>
-      <c r="B29" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
+      <c r="B29" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="n">

</xml_diff>

<commit_message>
plano de aulas + publicar aulas
</commit_message>
<xml_diff>
--- a/content/plano-de-aulas.xlsx
+++ b/content/plano-de-aulas.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="103">
   <si>
     <t xml:space="preserve">Data</t>
   </si>
@@ -58,6 +58,9 @@
     <t xml:space="preserve">Expositiva: Introdução ao curso
 Prática: escrever algoritmos simples com pseudo-código
 Java: usar cheatsheet para converter pseudo-código para Java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OK</t>
   </si>
   <si>
     <t xml:space="preserve">Como implementar ideia a partir do pseudo-código </t>
@@ -90,9 +93,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Rever testes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Comparando desempenho de algoritmos</t>
   </si>
   <si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t xml:space="preserve">Dá para resolver direto? Grupos de alunos fazem heurística para solução e depois trocam. Cada grupo agora deve encontrar uma entrada que quebra a heurística do outro.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rever testes</t>
   </si>
   <si>
     <t xml:space="preserve">Mochila binária II</t>
@@ -450,7 +453,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,6 +482,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.3999"/>
         <bgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFBBE33D"/>
+        <bgColor rgb="FFFFD966"/>
       </patternFill>
     </fill>
     <fill>
@@ -576,7 +585,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -601,6 +610,10 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -609,19 +622,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -633,7 +646,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -653,7 +666,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -661,7 +674,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -669,7 +682,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -733,7 +746,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFBBE33D"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -931,8 +944,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -994,6 +1007,9 @@
       <c r="F2" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="G2" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="n">
@@ -1006,33 +1022,35 @@
         <v>7</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="n">
         <f aca="false">A2+7</f>
         <v>45518</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="7"/>
       <c r="C4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="7" t="s">
         <v>14</v>
       </c>
+      <c r="D4" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="E4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="F4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
@@ -1042,21 +1060,19 @@
       <c r="B5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="E5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>19</v>
       </c>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
@@ -1066,21 +1082,19 @@
       <c r="B6" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="E6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>19</v>
-      </c>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
@@ -1102,9 +1116,7 @@
       <c r="F7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>19</v>
-      </c>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
@@ -1126,9 +1138,7 @@
       <c r="F8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>19</v>
-      </c>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="65.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
@@ -1150,9 +1160,7 @@
       <c r="F9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>19</v>
-      </c>
+      <c r="G9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
@@ -1162,20 +1170,20 @@
       <c r="B10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="8" t="s">
+      <c r="E10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>19</v>
+      <c r="G10" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="99.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1186,20 +1194,20 @@
       <c r="B11" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="D11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="E11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>34</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1211,16 +1219,16 @@
         <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1228,34 +1236,34 @@
         <f aca="false">A11+7</f>
         <v>45548</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="81.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="n">
         <f aca="false">A12+7</f>
         <v>45553</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="103.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
@@ -1265,20 +1273,20 @@
       <c r="B15" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="8" t="s">
+      <c r="D15" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="11" t="s">
-        <v>40</v>
+      <c r="E15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1289,20 +1297,20 @@
       <c r="B16" s="10" t="n">
         <v>12</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="12" t="s">
         <v>41</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G16" s="11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1313,20 +1321,20 @@
       <c r="B17" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="8" t="s">
+      <c r="C17" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="8" t="s">
+      <c r="D17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="E17" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>47</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1337,17 +1345,17 @@
       <c r="B18" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="8" t="s">
+      <c r="C18" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>49</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="98.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1358,20 +1366,20 @@
       <c r="B19" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="8" t="s">
+      <c r="C19" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="112.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1382,17 +1390,17 @@
       <c r="B20" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>50</v>
+      <c r="C20" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="99.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1403,17 +1411,17 @@
       <c r="B21" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="8" t="s">
+      <c r="C21" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>52</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="112.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1424,17 +1432,17 @@
       <c r="B22" s="10" t="n">
         <v>18</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="8" t="s">
+      <c r="C22" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>52</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="106.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1445,20 +1453,20 @@
       <c r="B23" s="10" t="n">
         <v>19</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="8" t="s">
+      <c r="C23" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="G23" s="9" t="s">
+      <c r="E23" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="9" t="s">
         <v>53</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="94" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1469,17 +1477,17 @@
       <c r="B24" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="C24" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>50</v>
+      <c r="C24" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1490,20 +1498,20 @@
       <c r="B25" s="10" t="n">
         <v>21</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>14</v>
+      <c r="C25" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G25" s="9" t="s">
+      <c r="F25" s="8" t="s">
         <v>56</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1514,17 +1522,17 @@
       <c r="B26" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="C26" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>14</v>
+      <c r="C26" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F26" s="7" t="s">
-        <v>57</v>
+      <c r="F26" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1535,17 +1543,17 @@
       <c r="B27" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="C27" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>58</v>
+      <c r="C27" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="7" t="s">
-        <v>59</v>
+      <c r="F27" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1556,17 +1564,17 @@
       <c r="B28" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="C28" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="8" t="s">
+      <c r="C28" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="14" t="s">
+      <c r="D28" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="E28" s="15" t="s">
         <v>38</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1574,30 +1582,30 @@
         <f aca="false">A27+7</f>
         <v>45604</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="n">
         <f aca="false">A28+7</f>
         <v>45609</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1671,7 +1679,7 @@
       <c r="B2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -1691,17 +1699,17 @@
       <c r="B3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1709,17 +1717,17 @@
         <f aca="false">A2+7</f>
         <v>45336</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" s="6"/>
+      <c r="D4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
@@ -1729,17 +1737,17 @@
       <c r="B5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="16" t="s">
         <v>14</v>
       </c>
+      <c r="D5" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="E5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>15</v>
+      <c r="F5" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1750,17 +1758,17 @@
       <c r="B6" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="15" t="s">
         <v>17</v>
       </c>
+      <c r="D6" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="E6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>18</v>
+      <c r="F6" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1771,16 +1779,16 @@
       <c r="B7" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1792,17 +1800,17 @@
       <c r="B8" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>14</v>
+      <c r="C8" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>55</v>
+      <c r="F8" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="155.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1813,17 +1821,17 @@
       <c r="B9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>14</v>
+      <c r="C9" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>57</v>
+      <c r="F9" s="8" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1834,17 +1842,17 @@
       <c r="B10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>58</v>
+      <c r="C10" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>59</v>
+      <c r="F10" s="8" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="99.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1855,17 +1863,17 @@
       <c r="B11" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>14</v>
+      <c r="C11" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>64</v>
+      <c r="F11" s="9" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1876,16 +1884,16 @@
       <c r="B12" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1894,17 +1902,17 @@
         <f aca="false">A11+7</f>
         <v>45366</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="14" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1913,18 +1921,18 @@
         <f aca="false">A12+7</f>
         <v>45371</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="8" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="15" t="s">
         <v>36</v>
       </c>
+      <c r="D14" s="9" t="s">
+        <v>37</v>
+      </c>
       <c r="E14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="8" t="s">
         <v>38</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="103.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1935,16 +1943,16 @@
       <c r="B15" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="12"/>
+      <c r="C15" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
@@ -1954,16 +1962,16 @@
       <c r="B16" s="10" t="n">
         <v>12</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="12"/>
+      <c r="C16" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="n">
@@ -1973,16 +1981,16 @@
       <c r="B17" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="6"/>
+      <c r="D17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="n">
@@ -1992,16 +2000,16 @@
       <c r="B18" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="9" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2013,17 +2021,17 @@
       <c r="B19" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>65</v>
+      <c r="D19" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>66</v>
+      <c r="F19" s="9" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2034,17 +2042,17 @@
       <c r="B20" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>41</v>
+      <c r="C20" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2055,17 +2063,17 @@
       <c r="B21" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="8" t="s">
+      <c r="C21" s="15" t="s">
         <v>45</v>
       </c>
+      <c r="D21" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="E21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>46</v>
+      <c r="F21" s="9" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="94" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2076,17 +2084,17 @@
       <c r="B22" s="10" t="n">
         <v>18</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>48</v>
+      <c r="C22" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="8" t="s">
-        <v>49</v>
+      <c r="F22" s="9" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2097,17 +2105,17 @@
       <c r="B23" s="10" t="n">
         <v>19</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>50</v>
+      <c r="C23" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>50</v>
+      <c r="F23" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="94" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2118,17 +2126,17 @@
       <c r="B24" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="C24" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>51</v>
+      <c r="C24" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>52</v>
+      <c r="F24" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2139,17 +2147,17 @@
       <c r="B25" s="10" t="n">
         <v>21</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>50</v>
+      <c r="C25" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="8" t="s">
-        <v>50</v>
+      <c r="F25" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2160,16 +2168,16 @@
       <c r="B26" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" s="6" t="s">
+      <c r="C26" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="6"/>
+      <c r="D26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="n">
@@ -2179,16 +2187,16 @@
       <c r="B27" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="8" t="s">
         <v>30</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="8" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2200,17 +2208,17 @@
       <c r="B28" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>32</v>
+      <c r="D28" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F28" s="7" t="s">
-        <v>33</v>
+      <c r="F28" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2218,30 +2226,30 @@
         <f aca="false">A27+7</f>
         <v>45422</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="n">
         <f aca="false">A28+7</f>
         <v>45427</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2315,7 +2323,7 @@
       <c r="B2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -2335,17 +2343,17 @@
       <c r="B3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2353,17 +2361,17 @@
         <f aca="false">A2+7</f>
         <v>45336</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="6" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F4" s="6"/>
+      <c r="D4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="n">
@@ -2373,20 +2381,20 @@
       <c r="B5" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>67</v>
+        <v>13</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2397,17 +2405,17 @@
       <c r="B6" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>68</v>
+      <c r="C6" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>69</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>69</v>
+      <c r="F6" s="9" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2418,17 +2426,17 @@
       <c r="B7" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="15" t="s">
         <v>17</v>
       </c>
+      <c r="D7" s="9" t="s">
+        <v>18</v>
+      </c>
       <c r="E7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>70</v>
+      <c r="F7" s="9" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="144.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2439,17 +2447,17 @@
       <c r="B8" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>71</v>
+      <c r="C8" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>72</v>
+      <c r="F8" s="9" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="155.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2460,17 +2468,17 @@
       <c r="B9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>14</v>
+      <c r="C9" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>15</v>
+      <c r="F9" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2481,17 +2489,17 @@
       <c r="B10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>14</v>
+      <c r="C10" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>74</v>
+      <c r="F10" s="8" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="88.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2502,17 +2510,17 @@
       <c r="B11" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>58</v>
+      <c r="C11" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>59</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>75</v>
+      <c r="F11" s="8" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2523,17 +2531,17 @@
       <c r="B12" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>14</v>
+      <c r="C12" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>15</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>77</v>
+      <c r="F12" s="9" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="74.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2541,17 +2549,17 @@
         <f aca="false">A11+7</f>
         <v>45366</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="14" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="9" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2560,21 +2568,21 @@
         <f aca="false">A12+7</f>
         <v>45371</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="14" t="s">
+      <c r="B14" s="13"/>
+      <c r="C14" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="103.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2585,16 +2593,16 @@
       <c r="B15" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="12"/>
+      <c r="C15" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
@@ -2604,27 +2612,27 @@
       <c r="B16" s="10" t="n">
         <v>12</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="12"/>
+      <c r="C16" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="13"/>
       <c r="I16" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="J16" s="15" t="s">
-        <v>79</v>
+      <c r="J16" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2635,16 +2643,16 @@
       <c r="B17" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="6"/>
+      <c r="D17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="n">
@@ -2654,16 +2662,16 @@
       <c r="B18" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="9" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2675,17 +2683,17 @@
       <c r="B19" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>65</v>
+      <c r="D19" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>66</v>
+      <c r="F19" s="9" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2696,17 +2704,17 @@
       <c r="B20" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>41</v>
+      <c r="C20" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2717,17 +2725,17 @@
       <c r="B21" s="10" t="n">
         <v>17</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="8" t="s">
+      <c r="C21" s="15" t="s">
         <v>45</v>
       </c>
+      <c r="D21" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="E21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>46</v>
+      <c r="F21" s="9" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2738,20 +2746,20 @@
       <c r="B22" s="10" t="n">
         <v>18</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>48</v>
+      <c r="C22" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>67</v>
+      <c r="F22" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2762,17 +2770,17 @@
       <c r="B23" s="10" t="n">
         <v>19</v>
       </c>
-      <c r="C23" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>50</v>
+      <c r="C23" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>50</v>
+      <c r="F23" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2783,17 +2791,17 @@
       <c r="B24" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="C24" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>51</v>
+      <c r="C24" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F24" s="8" t="s">
-        <v>52</v>
+      <c r="F24" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2804,20 +2812,20 @@
       <c r="B25" s="10" t="n">
         <v>21</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>50</v>
+      <c r="C25" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>67</v>
+      <c r="F25" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="79.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2828,16 +2836,16 @@
       <c r="B26" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" s="6" t="s">
+      <c r="C26" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="6"/>
+      <c r="D26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="89.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="n">
@@ -2847,16 +2855,16 @@
       <c r="B27" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="8" t="s">
         <v>30</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="8" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2868,20 +2876,20 @@
       <c r="B28" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>32</v>
+      <c r="D28" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F28" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G28" s="17" t="s">
-        <v>82</v>
+      <c r="F28" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G28" s="18" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2889,30 +2897,30 @@
         <f aca="false">A27+7</f>
         <v>45422</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="n">
         <f aca="false">A28+7</f>
         <v>45427</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2983,7 +2991,7 @@
       <c r="B2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -3000,12 +3008,12 @@
       <c r="B3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="8"/>
       <c r="D3" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3016,15 +3024,15 @@
       <c r="B4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="8"/>
       <c r="D4" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="18" t="s">
-        <v>83</v>
+        <v>13</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3035,14 +3043,14 @@
       <c r="B5" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="8" t="s">
+      <c r="C5" s="20" t="s">
         <v>85</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3050,12 +3058,12 @@
         <f aca="false">A4+7</f>
         <v>44979</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="B6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
@@ -3065,12 +3073,12 @@
       <c r="B7" s="10" t="n">
         <v>5</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" s="8" t="s">
+      <c r="C7" s="20"/>
+      <c r="D7" s="9" t="s">
         <v>87</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="102" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3081,12 +3089,12 @@
       <c r="B8" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="8" t="s">
+      <c r="C8" s="20"/>
+      <c r="D8" s="9" t="s">
         <v>89</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="155.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3097,14 +3105,14 @@
       <c r="B9" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="C9" s="20" t="s">
-        <v>90</v>
+      <c r="C9" s="21" t="s">
+        <v>91</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="101.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3115,12 +3123,12 @@
       <c r="B10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="88.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3131,13 +3139,13 @@
       <c r="B11" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="C11" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3149,11 +3157,11 @@
       <c r="B12" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="8" t="s">
+      <c r="C12" s="22"/>
+      <c r="D12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="9" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3165,11 +3173,11 @@
       <c r="B13" s="10" t="n">
         <v>11</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="8" t="s">
+      <c r="C13" s="22"/>
+      <c r="D13" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="9" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3178,24 +3186,24 @@
         <f aca="false">A12+7</f>
         <v>45007</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
+      <c r="B14" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
     </row>
     <row r="15" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
         <f aca="false">A13+7</f>
         <v>45009</v>
       </c>
-      <c r="B15" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
+      <c r="B15" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
     </row>
     <row r="16" customFormat="false" ht="79.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
@@ -3205,29 +3213,29 @@
       <c r="B16" s="10" t="n">
         <v>12</v>
       </c>
-      <c r="C16" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="8" t="s">
+      <c r="C16" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>15</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="H16" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="I16" s="15" t="s">
-        <v>79</v>
+      <c r="I16" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="L16" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="L16" s="19" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="93" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3238,12 +3246,12 @@
       <c r="B17" s="10" t="n">
         <v>13</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>94</v>
+      <c r="C17" s="20"/>
+      <c r="D17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3251,24 +3259,24 @@
         <f aca="false">A16+7</f>
         <v>45021</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="B18" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="n">
         <f aca="false">A17+7</f>
         <v>45023</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="B19" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="72.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="n">
@@ -3278,15 +3286,15 @@
       <c r="B20" s="10" t="n">
         <v>14</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>83</v>
+      <c r="C20" s="20"/>
+      <c r="D20" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3297,14 +3305,14 @@
       <c r="B21" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>96</v>
+      <c r="C21" s="8" t="s">
+        <v>97</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3315,12 +3323,12 @@
       <c r="B22" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="C22" s="7"/>
+      <c r="C22" s="8"/>
       <c r="D22" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3328,12 +3336,12 @@
         <f aca="false">A21+7</f>
         <v>45037</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
+      <c r="B23" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="n">
@@ -3343,12 +3351,12 @@
       <c r="B24" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="C24" s="7"/>
+      <c r="C24" s="8"/>
       <c r="D24" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3359,12 +3367,12 @@
       <c r="B25" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="C25" s="7"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3375,13 +3383,13 @@
       <c r="B26" s="10" t="n">
         <v>19</v>
       </c>
-      <c r="C26" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" s="8" t="s">
+      <c r="C26" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3393,10 +3401,10 @@
       <c r="B27" s="10" t="n">
         <v>20</v>
       </c>
-      <c r="C27" s="21"/>
+      <c r="C27" s="22"/>
       <c r="D27" s="10"/>
-      <c r="E27" s="8" t="s">
-        <v>33</v>
+      <c r="E27" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3407,10 +3415,10 @@
       <c r="B28" s="10" t="n">
         <v>21</v>
       </c>
-      <c r="C28" s="21"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="10"/>
-      <c r="E28" s="8" t="s">
-        <v>101</v>
+      <c r="E28" s="9" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3418,12 +3426,12 @@
         <f aca="false">A27+7</f>
         <v>45058</v>
       </c>
-      <c r="B29" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
+      <c r="B29" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="n">

</xml_diff>

<commit_message>
atualiza plano de aulas
</commit_message>
<xml_diff>
--- a/content/plano-de-aulas.xlsx
+++ b/content/plano-de-aulas.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t>Data</t>
   </si>
@@ -60,9 +60,6 @@
   <si>
     <t xml:space="preserve">Prática: resolver exercícios de intro a programação em Java. 
 Java: usar cheatsheet para converter pseudo-código para Java</t>
-  </si>
-  <si>
-    <t>REPOSICAO</t>
   </si>
   <si>
     <t xml:space="preserve">Algoritmos p3 - Busca em Strings</t>
@@ -109,16 +106,16 @@
 Implementação em Java: Bubblesort, insertion sort. Ref Cormen cap 2</t>
   </si>
   <si>
-    <t>Recursão</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Representando problemas usando recursão</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expositiva + exercícios de algoritmos recursivos</t>
+    <t xml:space="preserve">REPOSIÇÃO 2/24/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aula extra de implementação</t>
   </si>
   <si>
     <t>SIGCSE</t>
+  </si>
+  <si>
+    <t>FERIADO</t>
   </si>
   <si>
     <t xml:space="preserve">Ordenando rápido (na média)</t>
@@ -138,6 +135,9 @@
 Ref Cormen cap 7</t>
   </si>
   <si>
+    <t xml:space="preserve">REPOSICAO (11/03)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Otimizar escolha de ativos levando em conta budget</t>
   </si>
   <si>
@@ -195,15 +195,12 @@
   </si>
   <si>
     <t xml:space="preserve">Discussão: explorar problemas do algoritmo da aula passada
-Desenvolver algoritmo na lousa
+Desenvolver algoritmo DFS na lousa
 Aluno faz Implementação com testes de unidade
 Ref Cormen cap 22</t>
   </si>
   <si>
     <t xml:space="preserve">E o mais curto?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ref Cormen cap 22</t>
   </si>
   <si>
     <t xml:space="preserve">Discussão: explorar problemas do algoritmo da aula passada
@@ -213,10 +210,10 @@
 Ref Cormen cap 22</t>
   </si>
   <si>
-    <t xml:space="preserve">Problema para resolver no Labirinto</t>
-  </si>
-  <si>
     <t xml:space="preserve">Estruturas de Dados</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ref Cormen cap 22</t>
   </si>
   <si>
     <t xml:space="preserve">Implementações de algoritmos com tipo lista
@@ -242,13 +239,31 @@
     <t xml:space="preserve">Plano para aula na lousa</t>
   </si>
   <si>
+    <t>Recursão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Representando problemas usando recursão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expositiva + exercícios de algoritmos recursivos</t>
+  </si>
+  <si>
     <t xml:space="preserve">Criar do zero</t>
   </si>
   <si>
     <t xml:space="preserve">Encontrar problemas e listar no site. </t>
   </si>
   <si>
+    <t xml:space="preserve">Discussão: explorar problemas do algoritmo da aula passada
+Desenvolver algoritmo na lousa
+Aluno faz Implementação com testes de unidade
+Ref Cormen cap 22</t>
+  </si>
+  <si>
     <t xml:space="preserve">Revisão leve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problema para resolver no Labirinto</t>
   </si>
   <si>
     <t xml:space="preserve">Revisão leve → encontrar problemas leetcode para ajudar na prática</t>
@@ -507,7 +522,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -542,6 +557,18 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79990000000000006"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor rgb="FFC00000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor theme="7" tint="0.59999389629810485"/>
       </patternFill>
     </fill>
     <fill>
@@ -627,7 +654,7 @@
       <protection hidden="0" locked="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -646,9 +673,6 @@
     </xf>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="6" applyFont="1" applyFill="1" applyProtection="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -674,6 +698,9 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="6" applyFont="1" applyFill="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="3" fillId="3" borderId="1" numFmtId="0" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="0" locked="1"/>
@@ -686,24 +713,48 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="0" fillId="6" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="1">
+    <xf fontId="0" fillId="7" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="1">
+    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="9" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="8" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="11" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection hidden="0" locked="1"/>
+    </xf>
+    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection hidden="0" locked="1"/>
     </xf>
-    <xf fontId="0" fillId="10" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="1">
+    <xf fontId="0" fillId="12" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="2" fillId="2" borderId="0" numFmtId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -1233,7 +1284,7 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" topLeftCell="A10" zoomScale="100" workbookViewId="0">
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" topLeftCell="A22" zoomScale="100" workbookViewId="0">
       <selection activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
@@ -1248,6 +1299,7 @@
     <col customWidth="1" min="7" max="7" style="1" width="24.859999999999999"/>
     <col customWidth="1" min="8" max="8" style="1" width="18.579999999999998"/>
     <col customWidth="1" min="9" max="9" style="1" width="25.710000000000001"/>
+    <col customWidth="1" min="10" max="10" width="16.28125"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
@@ -1314,278 +1366,263 @@
       </c>
     </row>
     <row r="4" ht="85.5">
-      <c r="A4" s="6" t="s">
-        <v>12</v>
+      <c r="A4" s="3">
+        <f t="shared" ref="A4:A7" si="0">A2+7</f>
+        <v>45700</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="8"/>
+      <c r="G4" s="7"/>
     </row>
     <row r="5" ht="142.5">
       <c r="A5" s="3">
-        <f>A2+7</f>
-        <v>45700</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10" t="s">
+        <f t="shared" si="0"/>
+        <v>45702</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>17</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" ht="142.5">
       <c r="A6" s="3">
-        <f>A3+7</f>
-        <v>45702</v>
+        <f t="shared" si="0"/>
+        <v>45707</v>
       </c>
       <c r="B6" s="4">
         <v>3</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="10" t="s">
+    </row>
+    <row r="7" ht="99.75">
+      <c r="A7" s="3">
+        <f t="shared" si="0"/>
+        <v>45709</v>
+      </c>
+      <c r="B7" s="10">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" ht="142.5">
-      <c r="A7" s="3">
-        <f>A5+7</f>
-        <v>45707</v>
-      </c>
-      <c r="B7" s="11">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="D7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="5" t="s">
+    </row>
+    <row r="8" ht="57" customHeight="1">
+      <c r="A8" s="11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" ht="81.75" customHeight="1">
-      <c r="A8" s="3">
-        <f>A6+7</f>
-        <v>45709</v>
-      </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10"/>
+      <c r="C8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" ht="81.75" customHeight="1">
+      <c r="A9" s="3">
+        <f t="shared" ref="A9:A10" si="1">A6+7</f>
+        <v>45714</v>
+      </c>
+      <c r="B9" s="10">
         <v>5</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="C9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" ht="98.5" customHeight="1">
-      <c r="A9" s="3">
-        <f>A7+7</f>
-        <v>45714</v>
-      </c>
-      <c r="B9" s="11">
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" ht="98.5" customHeight="1">
+      <c r="A10" s="3">
+        <f t="shared" si="1"/>
+        <v>45716</v>
+      </c>
+      <c r="B10" s="10">
         <v>6</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-    </row>
-    <row r="10" ht="65.650000000000006" customHeight="1">
-      <c r="A10" s="3">
-        <f>A8+7</f>
-        <v>45716</v>
-      </c>
-      <c r="B10" s="4">
-        <v>7</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" ht="101.25" customHeight="1">
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" ht="65.650000000000006" customHeight="1">
       <c r="A11" s="3">
         <f>A9+7</f>
         <v>45721</v>
       </c>
       <c r="B11" s="4">
-        <v>8</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" ht="101.25" customHeight="1">
+      <c r="A12" s="1"/>
+      <c r="B12" s="4">
+        <v>8</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" ht="99.950000000000003" customHeight="1">
-      <c r="A12" s="3">
+    </row>
+    <row r="13" ht="99.950000000000003" customHeight="1">
+      <c r="A13" s="3">
         <f>A10+7</f>
         <v>45723</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="C13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="5" t="s">
+    </row>
+    <row r="14" ht="99.950000000000003" customHeight="1">
+      <c r="A14" s="12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="13" ht="99.950000000000003" customHeight="1">
-      <c r="A13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="10" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="10" t="s">
+      <c r="E14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" ht="75" customHeight="1">
-      <c r="A14" s="3">
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" ht="93.75" customHeight="1">
+      <c r="A15" s="3">
         <f>A11+7</f>
         <v>45728</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B15" s="10">
         <v>10</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="10" t="s">
+      <c r="E15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" ht="74.599999999999994" customHeight="1">
-      <c r="A15" s="3">
-        <f>A12+7</f>
+    <row r="16" ht="74.599999999999994" customHeight="1">
+      <c r="A16" s="3">
+        <f>A13+7</f>
         <v>45730</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="10" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10" t="s">
+      <c r="D16" s="9"/>
+      <c r="E16" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" ht="81.299999999999997" customHeight="1">
-      <c r="A16" s="3">
-        <f>A14+7</f>
+    <row r="17" ht="81.299999999999997" customHeight="1">
+      <c r="A17" s="3">
+        <f t="shared" ref="A17:A33" si="2">A15+7</f>
         <v>45735</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="5" t="s">
+      <c r="B17" s="13"/>
+      <c r="C17" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F17" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" ht="103.7" customHeight="1">
-      <c r="A17" s="3">
-        <f>A15+7</f>
+    <row r="18" ht="103.7" customHeight="1">
+      <c r="A18" s="3">
+        <f t="shared" si="2"/>
         <v>45737</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B18" s="10">
         <v>11</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" ht="79.5" customHeight="1">
-      <c r="A18" s="3">
-        <f>A16+7</f>
-        <v>45742</v>
-      </c>
-      <c r="B18" s="11">
-        <v>12</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>43</v>
@@ -1598,13 +1635,13 @@
       </c>
       <c r="F18" s="13"/>
     </row>
-    <row r="19" ht="93" customHeight="1">
+    <row r="19" ht="79.5" customHeight="1">
       <c r="A19" s="3">
-        <f>A17+7</f>
-        <v>45744</v>
-      </c>
-      <c r="B19" s="11">
-        <v>13</v>
+        <f t="shared" si="2"/>
+        <v>45742</v>
+      </c>
+      <c r="B19" s="10">
+        <v>12</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>43</v>
@@ -1617,271 +1654,280 @@
       </c>
       <c r="F19" s="13"/>
     </row>
-    <row r="20" ht="106.5" customHeight="1">
+    <row r="20" ht="93" customHeight="1">
       <c r="A20" s="3">
-        <f>A18+7</f>
+        <f t="shared" si="2"/>
+        <v>45744</v>
+      </c>
+      <c r="B20" s="10">
+        <v>13</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="13"/>
+    </row>
+    <row r="21" ht="106.5" customHeight="1">
+      <c r="A21" s="3">
+        <f t="shared" si="2"/>
         <v>45749</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B21" s="10">
         <v>14</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" ht="144.75" customHeight="1">
-      <c r="A21" s="3">
-        <f>A19+7</f>
-        <v>45751</v>
-      </c>
-      <c r="B21" s="4">
-        <v>15</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>47</v>
+      <c r="D21" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" ht="112.65000000000001" customHeight="1">
+      <c r="F21" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" ht="144.75" customHeight="1">
       <c r="A22" s="3">
-        <f>A20+7</f>
-        <v>45756</v>
-      </c>
-      <c r="B22" s="11">
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>45751</v>
+      </c>
+      <c r="B22" s="4">
+        <v>15</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="9" t="s">
         <v>47</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" ht="99.25" customHeight="1">
+      <c r="F22" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" ht="112.65000000000001" customHeight="1">
       <c r="A23" s="3">
-        <f>A21+7</f>
-        <v>45758</v>
-      </c>
-      <c r="B23" s="11">
-        <v>17</v>
+        <f t="shared" si="2"/>
+        <v>45756</v>
+      </c>
+      <c r="B23" s="10">
+        <v>16</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>50</v>
+      <c r="D23" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" ht="112.65000000000001" customHeight="1">
+      <c r="F23" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" ht="99.25" customHeight="1">
       <c r="A24" s="3">
-        <f>A22+7</f>
-        <v>45763</v>
-      </c>
-      <c r="B24" s="11">
-        <v>18</v>
+        <f t="shared" si="2"/>
+        <v>45758</v>
+      </c>
+      <c r="B24" s="10">
+        <v>17</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>50</v>
+      <c r="D24" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="E24" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" ht="106.7" customHeight="1">
+      <c r="F24" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" ht="112.65000000000001" customHeight="1">
       <c r="A25" s="3">
-        <f>A23+7</f>
-        <v>45765</v>
-      </c>
-      <c r="B25" s="11">
-        <v>19</v>
+        <f t="shared" si="2"/>
+        <v>45763</v>
+      </c>
+      <c r="B25" s="10">
+        <v>18</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="9" t="s">
         <v>50</v>
       </c>
       <c r="E25" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" ht="106.7" customHeight="1">
+      <c r="A26" s="3">
+        <f t="shared" si="2"/>
+        <v>45765</v>
+      </c>
+      <c r="B26" s="10">
+        <v>19</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+    </row>
+    <row r="27" ht="94" customHeight="1">
+      <c r="A27" s="3">
+        <f t="shared" si="2"/>
+        <v>45770</v>
+      </c>
+      <c r="B27" s="10">
+        <v>20</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" ht="55.950000000000003" customHeight="1">
+      <c r="A28" s="3">
+        <f t="shared" si="2"/>
+        <v>45772</v>
+      </c>
+      <c r="B28" s="10">
+        <v>21</v>
+      </c>
+      <c r="C28" s="18" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="26" ht="94" customHeight="1">
-      <c r="A26" s="3">
-        <f>A24+7</f>
-        <v>45770</v>
-      </c>
-      <c r="B26" s="11">
-        <v>20</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="10" t="s">
+      <c r="D28" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" ht="55.950000000000003" customHeight="1">
-      <c r="A27" s="3">
-        <f>A25+7</f>
-        <v>45772</v>
-      </c>
-      <c r="B27" s="11">
-        <v>21</v>
-      </c>
-      <c r="C27" s="16" t="s">
+    </row>
+    <row r="29" ht="79.099999999999994" customHeight="1">
+      <c r="A29" s="3">
+        <f t="shared" si="2"/>
+        <v>45777</v>
+      </c>
+      <c r="B29" s="4">
+        <v>22</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" ht="79.099999999999994" customHeight="1">
-      <c r="A28" s="3">
-        <f>A26+7</f>
-        <v>45777</v>
-      </c>
-      <c r="B28" s="4">
-        <v>22</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="7" t="s">
+    </row>
+    <row r="30" ht="89.549999999999997" customHeight="1">
+      <c r="A30" s="3">
+        <f t="shared" si="2"/>
+        <v>45779</v>
+      </c>
+      <c r="B30" s="4">
+        <v>23</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+    </row>
+    <row r="31" ht="69.400000000000006" customHeight="1">
+      <c r="A31" s="3">
+        <f t="shared" si="2"/>
+        <v>45784</v>
+      </c>
+      <c r="B31" s="4">
+        <v>24</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D31" s="21" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" ht="89.549999999999997" customHeight="1">
-      <c r="A29" s="3">
-        <f>A27+7</f>
-        <v>45779</v>
-      </c>
-      <c r="B29" s="4">
-        <v>23</v>
-      </c>
-      <c r="C29" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="7" t="s">
+      <c r="E31" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="30" ht="69.400000000000006" customHeight="1">
-      <c r="A30" s="3">
-        <f>A28+7</f>
-        <v>45784</v>
-      </c>
-      <c r="B30" s="4">
-        <v>24</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" ht="13.800000000000001" customHeight="1">
-      <c r="A31" s="3">
-        <f>A29+7</f>
+    </row>
+    <row r="32" ht="13.800000000000001" customHeight="1">
+      <c r="A32" s="3">
+        <f t="shared" si="2"/>
         <v>45786</v>
-      </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-    </row>
-    <row r="32" ht="14.25">
-      <c r="A32" s="3">
-        <f>A30+7</f>
-        <v>45791</v>
       </c>
       <c r="B32" s="13"/>
       <c r="C32" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
     </row>
-    <row r="1048576" ht="12.800000000000001"/>
+    <row r="33" ht="14.25">
+      <c r="A33" s="3">
+        <f t="shared" si="2"/>
+        <v>45791</v>
+      </c>
+      <c r="B33" s="13"/>
+      <c r="C33" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="C9:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C30:F30"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.51181102362204689" footer="0.51181102362204689"/>
@@ -1956,8 +2002,8 @@
       <c r="F2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="17" t="s">
-        <v>59</v>
+      <c r="G2" s="23" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3" ht="57">
@@ -1979,233 +2025,233 @@
       <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="17"/>
+      <c r="G3" s="23"/>
     </row>
     <row r="4" ht="85.5">
       <c r="A4" s="3">
-        <f t="shared" ref="A4:A11" si="0">A2+7</f>
+        <f t="shared" ref="A4:A11" si="3">A2+7</f>
         <v>45518</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="17"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" ht="142.5">
       <c r="A5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>45520</v>
       </c>
       <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="17"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" ht="142.5">
       <c r="A6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>45525</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>4</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="10" t="s">
+      <c r="C6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="17"/>
+      <c r="G6" s="23"/>
     </row>
     <row r="7" ht="99.75">
       <c r="A7" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>45527</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="17"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" ht="98.5" customHeight="1">
       <c r="A8" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>45532</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="17"/>
+      <c r="G8" s="23"/>
     </row>
     <row r="9" ht="65.650000000000006" customHeight="1">
       <c r="A9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>45534</v>
       </c>
       <c r="B9" s="4">
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="17"/>
+      <c r="G9" s="23"/>
     </row>
     <row r="10" ht="101.25" customHeight="1">
       <c r="A10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>45539</v>
       </c>
       <c r="B10" s="4">
         <v>8</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="E10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="18" t="s">
-        <v>60</v>
+      <c r="G10" s="24" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="11" ht="99.950000000000003" customHeight="1">
       <c r="A11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>45541</v>
       </c>
       <c r="B11" s="4">
         <v>9</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="10" t="s">
+      <c r="E11" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="19" t="s">
-        <v>61</v>
+      <c r="G11" s="25" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="12" ht="75" customHeight="1">
       <c r="A12" s="3">
-        <f t="shared" ref="A12:A30" si="1">A10+7</f>
+        <f t="shared" ref="A12:A30" si="4">A10+7</f>
         <v>45546</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <v>10</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>24</v>
+      <c r="C12" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="13" ht="74.599999999999994" customHeight="1">
       <c r="A13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45548</v>
       </c>
       <c r="B13" s="13"/>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="20" t="s">
-        <v>63</v>
+      <c r="G13" s="26" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="14" ht="81.299999999999997" customHeight="1">
       <c r="A14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45553</v>
       </c>
       <c r="B14" s="13"/>
@@ -2224,10 +2270,10 @@
     </row>
     <row r="15" ht="103.7" customHeight="1">
       <c r="A15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45555</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="10">
         <v>11</v>
       </c>
       <c r="C15" s="14" t="s">
@@ -2243,10 +2289,10 @@
     </row>
     <row r="16" ht="79.5" customHeight="1">
       <c r="A16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45560</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="10">
         <v>12</v>
       </c>
       <c r="C16" s="14" t="s">
@@ -2262,49 +2308,49 @@
     </row>
     <row r="17" ht="93" customHeight="1">
       <c r="A17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45562</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="10">
         <v>13</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>45</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="18" ht="128.25">
       <c r="A18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45567</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="10">
         <v>14</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>47</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="19" ht="98.5" customHeight="1">
       <c r="A19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45569</v>
       </c>
       <c r="B19" s="4">
@@ -2313,202 +2359,202 @@
       <c r="C19" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>47</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>64</v>
+      <c r="F19" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="20" ht="112.65000000000001" customHeight="1">
       <c r="A20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45574</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="10">
         <v>16</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>53</v>
+      <c r="D20" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F20" s="10" t="s">
-        <v>53</v>
+      <c r="F20" s="9" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="21" ht="99.25" customHeight="1">
       <c r="A21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45576</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="10">
         <v>17</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>50</v>
       </c>
       <c r="E21" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="10" t="s">
-        <v>51</v>
+      <c r="F21" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="22" ht="112.65000000000001" customHeight="1">
       <c r="A22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45581</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="10">
         <v>18</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="9" t="s">
         <v>50</v>
       </c>
       <c r="E22" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="10" t="s">
-        <v>52</v>
+      <c r="F22" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="23" ht="106.7" customHeight="1">
       <c r="A23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45583</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="10">
         <v>19</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="9" t="s">
         <v>50</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" s="18" t="s">
-        <v>65</v>
+      <c r="F23" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="24" ht="94" customHeight="1">
       <c r="A24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45588</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="10">
         <v>20</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="10" t="s">
-        <v>53</v>
+      <c r="D24" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="E24" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="10" t="s">
-        <v>53</v>
+      <c r="F24" s="9" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="25" ht="55.950000000000003" customHeight="1">
       <c r="A25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45590</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="10">
         <v>21</v>
       </c>
-      <c r="C25" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>14</v>
+      <c r="C25" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G25" s="21" t="s">
-        <v>66</v>
+      <c r="F25" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="27" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="26" ht="79.099999999999994" customHeight="1">
       <c r="A26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45595</v>
       </c>
       <c r="B26" s="4">
         <v>22</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G26" s="21" t="s">
-        <v>66</v>
+      <c r="G26" s="27" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="27" ht="89.549999999999997" customHeight="1">
       <c r="A27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45597</v>
       </c>
       <c r="B27" s="4">
         <v>23</v>
       </c>
-      <c r="C27" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D27" s="7" t="s">
+      <c r="C27" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G27" s="21" t="s">
-        <v>66</v>
+      <c r="G27" s="27" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="28" ht="69.400000000000006" customHeight="1">
       <c r="A28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45602</v>
       </c>
       <c r="B28" s="4">
@@ -2517,42 +2563,42 @@
       <c r="C28" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="9" t="s">
         <v>41</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="29" ht="13.800000000000001" customHeight="1">
       <c r="A29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45604</v>
       </c>
       <c r="B29" s="13"/>
       <c r="C29" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>45609</v>
       </c>
       <c r="B30" s="13"/>
       <c r="C30" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
@@ -2610,13 +2656,13 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" ht="57.450000000000003">
@@ -2626,7 +2672,7 @@
       <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -2646,7 +2692,7 @@
       <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -2661,233 +2707,233 @@
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="3">
-        <f t="shared" ref="A4:A11" si="2">A2+7</f>
+        <f t="shared" ref="A4:A11" si="5">A2+7</f>
         <v>45336</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="F4" s="9"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" ht="57.450000000000003">
       <c r="A5" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>45338</v>
       </c>
       <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="E5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>71</v>
+      <c r="F5" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="6" ht="113.40000000000001">
       <c r="A6" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>45343</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>4</v>
       </c>
       <c r="C6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>17</v>
-      </c>
       <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>72</v>
+      <c r="F6" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="7" ht="102.2">
       <c r="A7" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>45345</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>73</v>
+      <c r="F7" s="9" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="8" ht="144.75" customHeight="1">
       <c r="A8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>45350</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>6</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>14</v>
+      <c r="C8" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>74</v>
+      <c r="F8" s="6" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="9" ht="155.25" customHeight="1">
       <c r="A9" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>45352</v>
       </c>
       <c r="B9" s="4">
         <v>7</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="10" ht="101.25" customHeight="1">
       <c r="A10" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>45357</v>
       </c>
       <c r="B10" s="4">
         <v>8</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="11" ht="99.950000000000003" customHeight="1">
       <c r="A11" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>45359</v>
       </c>
       <c r="B11" s="4">
         <v>9</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>14</v>
+      <c r="C11" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="10" t="s">
-        <v>76</v>
+      <c r="F11" s="9" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="12" ht="75" customHeight="1">
       <c r="A12" s="3">
-        <f t="shared" ref="A12:A30" si="3">A10+7</f>
+        <f t="shared" ref="A12:A30" si="6">A10+7</f>
         <v>45364</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <v>10</v>
       </c>
       <c r="C12" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="E12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>77</v>
+      <c r="F12" s="9" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="13" ht="74.599999999999994" customHeight="1">
       <c r="A13" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45366</v>
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="10" t="s">
-        <v>78</v>
+      <c r="F13" s="9" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="14" ht="81.299999999999997" customHeight="1">
       <c r="A14" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45371</v>
       </c>
       <c r="B14" s="13"/>
       <c r="C14" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>41</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" ht="103.7" customHeight="1">
       <c r="A15" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45373</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="10">
         <v>11</v>
       </c>
       <c r="C15" s="14" t="s">
@@ -2903,10 +2949,10 @@
     </row>
     <row r="16" ht="79.5" customHeight="1">
       <c r="A16" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45378</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="10">
         <v>12</v>
       </c>
       <c r="C16" s="14" t="s">
@@ -2922,278 +2968,278 @@
     </row>
     <row r="17" ht="93" customHeight="1">
       <c r="A17" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45380</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="10">
         <v>13</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="9"/>
+      <c r="C17" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" ht="46.25">
       <c r="A18" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45385</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="10">
         <v>14</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="10" t="s">
-        <v>79</v>
+      <c r="F18" s="9" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="19" ht="23.850000000000001">
       <c r="A19" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45387</v>
       </c>
       <c r="B19" s="4">
         <v>15</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>80</v>
+        <v>20</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="10" t="s">
-        <v>81</v>
+      <c r="F19" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="20" ht="72.75" customHeight="1">
       <c r="A20" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45392</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="10">
         <v>16</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>24</v>
+      <c r="C20" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" ht="57.450000000000003">
       <c r="A21" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45394</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="10">
         <v>17</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>45</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="22" ht="94" customHeight="1">
       <c r="A22" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45399</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="10">
         <v>18</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="9" t="s">
         <v>47</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="10" t="s">
-        <v>82</v>
+      <c r="F22" s="9" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="23" ht="49.25" customHeight="1">
       <c r="A23" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45401</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="10">
         <v>19</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>53</v>
+      <c r="D23" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>53</v>
+      <c r="F23" s="9" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="24" ht="94" customHeight="1">
       <c r="A24" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45406</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="10">
         <v>20</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="9" t="s">
         <v>50</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="10" t="s">
-        <v>83</v>
+      <c r="F24" s="9" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="25" ht="55.950000000000003" customHeight="1">
       <c r="A25" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45408</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="10">
         <v>21</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>53</v>
+      <c r="D25" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="10" t="s">
-        <v>53</v>
+      <c r="F25" s="9" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="26" ht="79.099999999999994" customHeight="1">
       <c r="A26" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45413</v>
       </c>
       <c r="B26" s="4">
         <v>22</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="F26" s="9"/>
+      <c r="C26" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" s="8"/>
     </row>
     <row r="27" ht="89.549999999999997" customHeight="1">
       <c r="A27" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45415</v>
       </c>
       <c r="B27" s="4">
         <v>23</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="7" t="s">
-        <v>84</v>
+      <c r="F27" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="28" ht="69.400000000000006" customHeight="1">
       <c r="A28" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45420</v>
       </c>
       <c r="B28" s="4">
         <v>24</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>35</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="7" t="s">
-        <v>85</v>
+      <c r="F28" s="6" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="29" ht="13.800000000000001" customHeight="1">
       <c r="A29" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45422</v>
       </c>
       <c r="B29" s="13"/>
       <c r="C29" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>45427</v>
       </c>
       <c r="B30" s="13"/>
       <c r="C30" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
@@ -3251,13 +3297,13 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" ht="57.450000000000003">
@@ -3267,7 +3313,7 @@
       <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -3287,7 +3333,7 @@
       <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -3302,30 +3348,30 @@
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="3">
-        <f t="shared" ref="A4:A11" si="4">A2+7</f>
+        <f t="shared" ref="A4:A11" si="7">A2+7</f>
         <v>45336</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="F4" s="9"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" ht="46.25">
       <c r="A5" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>45338</v>
       </c>
       <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="5" t="s">
@@ -3337,204 +3383,204 @@
       <c r="F5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="23" t="s">
-        <v>86</v>
+      <c r="G5" s="29" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="6" ht="57.450000000000003">
       <c r="A6" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>45343</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>4</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>87</v>
+        <v>15</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="10" t="s">
-        <v>88</v>
+      <c r="F6" s="9" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="7" ht="79.849999999999994">
       <c r="A7" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>45345</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>5</v>
       </c>
       <c r="C7" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>17</v>
-      </c>
       <c r="E7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="10" t="s">
-        <v>89</v>
+      <c r="F7" s="9" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="8" ht="144.75" customHeight="1">
       <c r="A8" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>45350</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>6</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>90</v>
+        <v>15</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="10" t="s">
-        <v>91</v>
+      <c r="F8" s="9" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="9" ht="155.25" customHeight="1">
       <c r="A9" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>45352</v>
       </c>
       <c r="B9" s="4">
         <v>7</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>14</v>
+      <c r="C9" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>71</v>
+      <c r="F9" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="10" ht="101.25" customHeight="1">
       <c r="A10" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>45357</v>
       </c>
       <c r="B10" s="4">
         <v>8</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>14</v>
+      <c r="C10" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="7" t="s">
-        <v>93</v>
+      <c r="F10" s="6" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="11" ht="88.5" customHeight="1">
       <c r="A11" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>45359</v>
       </c>
       <c r="B11" s="4">
         <v>9</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>56</v>
+      <c r="C11" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>94</v>
+      <c r="F11" s="6" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="12" ht="75" customHeight="1">
       <c r="A12" s="3">
-        <f t="shared" ref="A12:A30" si="5">A10+7</f>
+        <f t="shared" ref="A12:A30" si="8">A10+7</f>
         <v>45364</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <v>10</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>14</v>
+      <c r="C12" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="10" t="s">
-        <v>96</v>
+      <c r="F12" s="9" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="13" ht="74.599999999999994" customHeight="1">
       <c r="A13" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45366</v>
       </c>
       <c r="B13" s="13"/>
       <c r="C13" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="E13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F13" s="10" t="s">
-        <v>77</v>
+      <c r="F13" s="9" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="14" ht="81.299999999999997" customHeight="1">
       <c r="A14" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45371</v>
       </c>
       <c r="B14" s="13"/>
       <c r="C14" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>27</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="10" t="s">
-        <v>78</v>
+      <c r="F14" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" ht="103.7" customHeight="1">
       <c r="A15" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45373</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="10">
         <v>11</v>
       </c>
       <c r="C15" s="14" t="s">
@@ -3550,10 +3596,10 @@
     </row>
     <row r="16" ht="79.5" customHeight="1">
       <c r="A16" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45378</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="10">
         <v>12</v>
       </c>
       <c r="C16" s="14" t="s">
@@ -3569,299 +3615,299 @@
       <c r="I16" s="4">
         <v>12</v>
       </c>
-      <c r="J16" s="16" t="s">
-        <v>98</v>
+      <c r="J16" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" ht="93" customHeight="1">
       <c r="A17" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45380</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="10">
         <v>13</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="9"/>
+      <c r="C17" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" s="8"/>
     </row>
     <row r="18" ht="46.25">
       <c r="A18" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45385</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="10">
         <v>14</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="10" t="s">
-        <v>79</v>
+      <c r="F18" s="9" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="19" ht="23.850000000000001">
       <c r="A19" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45387</v>
       </c>
       <c r="B19" s="4">
         <v>15</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>80</v>
+        <v>20</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="10" t="s">
-        <v>81</v>
+      <c r="F19" s="9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="20" ht="72.75" customHeight="1">
       <c r="A20" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45392</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="10">
         <v>16</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>24</v>
+      <c r="C20" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" ht="57.450000000000003">
       <c r="A21" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45394</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="10">
         <v>17</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>45</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="22" ht="41" customHeight="1">
       <c r="A22" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45399</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="10">
         <v>18</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="9" t="s">
         <v>47</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F22" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="G22" s="23" t="s">
+      <c r="F22" s="9" t="s">
         <v>86</v>
+      </c>
+      <c r="G22" s="29" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45401</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="10">
         <v>19</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="10" t="s">
-        <v>53</v>
+      <c r="D23" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="10" t="s">
-        <v>53</v>
+      <c r="F23" s="9" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="24" ht="39.549999999999997" customHeight="1">
       <c r="A24" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45406</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="10">
         <v>20</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="9" t="s">
         <v>50</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="10" t="s">
-        <v>83</v>
+      <c r="F24" s="9" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="25" ht="42.5" customHeight="1">
       <c r="A25" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45408</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="10">
         <v>21</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="10" t="s">
-        <v>53</v>
+      <c r="D25" s="9" t="s">
+        <v>68</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G25" s="23" t="s">
-        <v>86</v>
+      <c r="F25" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G25" s="29" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="26" ht="79.099999999999994" customHeight="1">
       <c r="A26" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45413</v>
       </c>
       <c r="B26" s="4">
         <v>22</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="F26" s="9"/>
+      <c r="C26" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" s="8"/>
     </row>
     <row r="27" ht="89.549999999999997" customHeight="1">
       <c r="A27" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45415</v>
       </c>
       <c r="B27" s="4">
         <v>23</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C27" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>33</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F27" s="7" t="s">
-        <v>84</v>
+      <c r="F27" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="28" ht="69.400000000000006" customHeight="1">
       <c r="A28" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45420</v>
       </c>
       <c r="B28" s="4">
         <v>24</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>35</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F28" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="G28" s="23" t="s">
-        <v>101</v>
+      <c r="F28" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G28" s="29" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="29" ht="13.800000000000001" customHeight="1">
       <c r="A29" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45422</v>
       </c>
       <c r="B29" s="13"/>
       <c r="C29" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>45427</v>
       </c>
       <c r="B30" s="13"/>
       <c r="C30" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
@@ -3916,13 +3962,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" ht="57.450000000000003">
@@ -3932,7 +3978,7 @@
       <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -3949,7 +3995,7 @@
       <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="6"/>
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
@@ -3959,295 +4005,295 @@
     </row>
     <row r="4" ht="46.25">
       <c r="A4" s="3">
-        <f t="shared" ref="A4:A11" si="6">A2+7</f>
+        <f t="shared" ref="A4:A11" si="9">A2+7</f>
         <v>44972</v>
       </c>
       <c r="B4" s="4">
         <v>3</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="6"/>
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="24" t="s">
-        <v>102</v>
+      <c r="F4" s="30" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="5" ht="23.850000000000001">
       <c r="A5" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>44974</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>4</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>104</v>
+      <c r="C5" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>44979</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="B6" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" ht="23.850000000000001">
       <c r="A7" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>44981</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>5</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>106</v>
+      <c r="C7" s="31"/>
+      <c r="D7" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="8" ht="102" customHeight="1">
       <c r="A8" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>44986</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>6</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>108</v>
+      <c r="C8" s="31"/>
+      <c r="D8" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="9" ht="155.25" customHeight="1">
       <c r="A9" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>44988</v>
       </c>
       <c r="B9" s="4">
         <v>7</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>109</v>
+      <c r="C9" s="18" t="s">
+        <v>113</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" ht="101.25" customHeight="1">
       <c r="A10" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>44993</v>
       </c>
       <c r="B10" s="4">
         <v>8</v>
       </c>
-      <c r="C10" s="16"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="5" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" ht="88.5" customHeight="1">
       <c r="A11" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>44995</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <v>9</v>
       </c>
       <c r="C11" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>77</v>
+      <c r="E11" s="9" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="12" ht="75" customHeight="1">
       <c r="A12" s="3">
-        <f t="shared" ref="A12:A33" si="7">A10+7</f>
+        <f t="shared" ref="A12:A33" si="10">A10+7</f>
         <v>45000</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <v>10</v>
       </c>
       <c r="C12" s="15"/>
-      <c r="D12" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>78</v>
+      <c r="D12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="13" ht="46.25">
       <c r="A13" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45002</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="10">
         <v>11</v>
       </c>
       <c r="C13" s="15"/>
-      <c r="D13" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>79</v>
+      <c r="D13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="14" ht="22.5" customHeight="1">
       <c r="A14" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45007</v>
       </c>
-      <c r="B14" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
+      <c r="B14" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
     </row>
     <row r="15" ht="22.5" customHeight="1">
       <c r="A15" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45009</v>
       </c>
-      <c r="B15" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
+      <c r="B15" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
     </row>
     <row r="16" ht="79.5" customHeight="1">
       <c r="A16" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45014</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="10">
         <v>12</v>
       </c>
-      <c r="C16" s="25" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>71</v>
+      <c r="C16" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>75</v>
       </c>
       <c r="H16" s="4">
         <v>12</v>
       </c>
-      <c r="I16" s="16" t="s">
-        <v>98</v>
+      <c r="I16" s="18" t="s">
+        <v>102</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="K16" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="L16" s="24" t="s">
-        <v>102</v>
+        <v>104</v>
+      </c>
+      <c r="L16" s="30" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="17" ht="93" customHeight="1">
       <c r="A17" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45016</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="10">
         <v>13</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="27" t="s">
-        <v>113</v>
+      <c r="C17" s="31"/>
+      <c r="D17" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45021</v>
       </c>
-      <c r="B18" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
+      <c r="B18" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45023</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
+      <c r="B19" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" ht="72.75" customHeight="1">
       <c r="A20" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45028</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="10">
         <v>14</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>102</v>
+      <c r="C20" s="31"/>
+      <c r="D20" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="21" ht="57.450000000000003">
       <c r="A21" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45030</v>
       </c>
       <c r="B21" s="4">
         <v>15</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>115</v>
+      <c r="C21" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>45</v>
@@ -4258,143 +4304,143 @@
     </row>
     <row r="22" ht="79.849999999999994">
       <c r="A22" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45035</v>
       </c>
       <c r="B22" s="4">
         <v>16</v>
       </c>
-      <c r="C22" s="7"/>
+      <c r="C22" s="6"/>
       <c r="D22" s="5" t="s">
         <v>47</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45037</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
+      <c r="B23" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
     </row>
     <row r="24" ht="79.849999999999994">
       <c r="A24" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45042</v>
       </c>
       <c r="B24" s="4">
         <v>17</v>
       </c>
-      <c r="C24" s="7"/>
+      <c r="C24" s="6"/>
       <c r="D24" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" ht="35.049999999999997">
       <c r="A25" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45044</v>
       </c>
       <c r="B25" s="4">
         <v>18</v>
       </c>
-      <c r="C25" s="7"/>
+      <c r="C25" s="6"/>
       <c r="D25" s="5" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" ht="57.450000000000003" customHeight="1">
       <c r="A26" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45049</v>
       </c>
-      <c r="B26" s="11">
+      <c r="B26" s="10">
         <v>19</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="D26" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="10" t="s">
-        <v>84</v>
+      <c r="E26" s="9" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="27" ht="57.450000000000003">
       <c r="A27" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45051</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B27" s="10">
         <v>20</v>
       </c>
       <c r="C27" s="15"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="10" t="s">
-        <v>85</v>
+      <c r="D27" s="10"/>
+      <c r="E27" s="9" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="28" ht="35.049999999999997">
       <c r="A28" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45056</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28" s="10">
         <v>21</v>
       </c>
       <c r="C28" s="15"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="10" t="s">
-        <v>120</v>
+      <c r="D28" s="10"/>
+      <c r="E28" s="9" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45058</v>
       </c>
-      <c r="B29" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
+      <c r="B29" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45063</v>
       </c>
     </row>
     <row r="31" ht="14.25">
       <c r="A31" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45065</v>
       </c>
     </row>
     <row r="32" ht="14.25">
       <c r="A32" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45070</v>
       </c>
     </row>
     <row r="33" ht="14.25">
       <c r="A33" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>45072</v>
       </c>
     </row>

</xml_diff>